<commit_message>
FInal and fully functionnal version of the experiment
</commit_message>
<xml_diff>
--- a/ParallelBotsExecution/FormFilling/Test-cases.xlsx
+++ b/ParallelBotsExecution/FormFilling/Test-cases.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\csharp\parallele-rpa-processes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\csharp\parallele-rpa-processes\ParallelBotsExecution\FormFilling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F61B040-4AA1-48D9-A937-4BA10C974697}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F32CC3-C058-484F-987B-2EF2A53D7096}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="6735" xr2:uid="{24CDF72B-4CAD-4959-B574-2BC8DCD2E34D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Cases" sheetId="1" r:id="rId1"/>
+    <sheet name="Results" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="21">
   <si>
     <t>First name</t>
   </si>
@@ -70,12 +71,42 @@
   </si>
   <si>
     <t>Bot status</t>
+  </si>
+  <si>
+    <t>Nb
+Chrome</t>
+  </si>
+  <si>
+    <t>Nb 
+lines</t>
+  </si>
+  <si>
+    <t>Normal
+Time</t>
+  </si>
+  <si>
+    <t>Normal
+Time per line
+(in seconds)</t>
+  </si>
+  <si>
+    <t>Headless 
+Time</t>
+  </si>
+  <si>
+    <t>Headless 
+Time per line
+(in seconds)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="167" formatCode="mm/yy"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -105,16 +136,51 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="9">
     <dxf>
-      <numFmt numFmtId="21" formatCode="dd\-mmm"/>
+      <numFmt numFmtId="167" formatCode="mm/yy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -130,8 +196,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{49999785-46C6-475A-B85F-87A36B0FA5B6}" name="Table1" displayName="Table1" ref="A1:M20" totalsRowShown="0">
-  <autoFilter ref="A1:M20" xr:uid="{10CA4C59-E48D-469A-863A-0312D013B7D3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{49999785-46C6-475A-B85F-87A36B0FA5B6}" name="Table1" displayName="Table1" ref="A1:M21" totalsRowShown="0">
+  <autoFilter ref="A1:M21" xr:uid="{10CA4C59-E48D-469A-863A-0312D013B7D3}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{5E333834-D29F-408B-B7C6-9FBC295B8569}" name="#"/>
     <tableColumn id="2" xr3:uid="{8CBCD003-8084-4DEA-92E7-AF5D8C500316}" name="First name">
@@ -160,6 +226,21 @@
       <calculatedColumnFormula>A2*100</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="13" xr3:uid="{097480AA-BE6F-4A26-8914-3ACB749445FF}" name="Bot status"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8F1A6880-8BD0-4FB4-975B-E723ACA35801}" name="Table13" displayName="Table13" ref="A1:F11" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A1:F11" xr:uid="{0865E496-69C6-4C70-9EA9-BA396D8E8B41}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{D48F6564-ADB0-4C1B-962E-584C9C9A0600}" name="Nb_x000a_Chrome" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{49597B0D-E449-42C0-957C-FF560E23C701}" name="Nb _x000a_lines" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{E6DA5C4C-5D98-4229-8CF1-B49BD6CC9EF4}" name="Normal_x000a_Time" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{24381721-47FD-4D99-AC28-70C780CF8496}" name="Normal_x000a_Time per line_x000a_(in seconds)" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{4C079BB4-A124-4E22-82AF-D38BA9185703}" name="Headless _x000a_Time" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{A260A3EE-2A2C-4374-A5CC-6DAA699EA4A1}" name="Headless _x000a_Time per line_x000a_(in seconds)" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -462,9 +543,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E45A287-3ADC-4ECF-A560-4D617666F00A}">
-  <dimension ref="A1:M20"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -475,7 +558,7 @@
     <col min="6" max="6" width="9.33203125" customWidth="1"/>
     <col min="9" max="9" width="14.1328125" customWidth="1"/>
     <col min="10" max="10" width="18.6640625" customWidth="1"/>
-    <col min="11" max="11" width="11.19921875" customWidth="1"/>
+    <col min="11" max="11" width="11.19921875" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.45">
@@ -509,7 +592,7 @@
       <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="5" t="s">
         <v>9</v>
       </c>
       <c r="L1" t="s">
@@ -528,15 +611,15 @@
         <v>First name 1</v>
       </c>
       <c r="C2" t="str">
-        <f t="shared" ref="C2:E17" si="0">_xlfn.CONCAT(C$1," ",$A2)</f>
+        <f>_xlfn.CONCAT(C$1," ",$A2)</f>
         <v>Last name 1</v>
       </c>
       <c r="D2" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(D$1," ",$A2)</f>
         <v>Username 1</v>
       </c>
       <c r="E2" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(E$1," ",$A2)</f>
         <v>Address 1</v>
       </c>
       <c r="F2" t="s">
@@ -556,7 +639,7 @@
         <f>A2*5662763</f>
         <v>5662763</v>
       </c>
-      <c r="K2" s="1">
+      <c r="K2" s="5">
         <v>43383</v>
       </c>
       <c r="L2">
@@ -569,19 +652,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="str">
-        <f t="shared" ref="B3:E20" si="1">_xlfn.CONCAT(B$1," ",$A3)</f>
+        <f>_xlfn.CONCAT(B$1," ",$A3)</f>
         <v>First name 2</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C$1," ",$A3)</f>
         <v>Last name 2</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(D$1," ",$A3)</f>
         <v>Username 2</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(E$1," ",$A3)</f>
         <v>Address 2</v>
       </c>
       <c r="F3" t="s">
@@ -594,18 +677,18 @@
         <v>6652</v>
       </c>
       <c r="I3" t="str">
-        <f t="shared" ref="I3:I20" si="2">_xlfn.CONCAT(C3," ",B3)</f>
+        <f t="shared" ref="I3:I20" si="0">_xlfn.CONCAT(C3," ",B3)</f>
         <v>Last name 2 First name 2</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J20" si="3">A3*5662763</f>
+        <f t="shared" ref="J3:J20" si="1">A3*5662763</f>
         <v>11325526</v>
       </c>
-      <c r="K3" s="1">
+      <c r="K3" s="5">
         <v>43384</v>
       </c>
       <c r="L3">
-        <f t="shared" ref="L3:L20" si="4">A3*100</f>
+        <f t="shared" ref="L3:L20" si="2">A3*100</f>
         <v>200</v>
       </c>
     </row>
@@ -614,19 +697,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(B$1," ",$A4)</f>
         <v>First name 3</v>
       </c>
       <c r="C4" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C$1," ",$A4)</f>
         <v>Last name 3</v>
       </c>
       <c r="D4" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(D$1," ",$A4)</f>
         <v>Username 3</v>
       </c>
       <c r="E4" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(E$1," ",$A4)</f>
         <v>Address 3</v>
       </c>
       <c r="F4" t="s">
@@ -639,18 +722,18 @@
         <v>6653</v>
       </c>
       <c r="I4" t="str">
+        <f t="shared" si="0"/>
+        <v>Last name 3 First name 3</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="1"/>
+        <v>16988289</v>
+      </c>
+      <c r="K4" s="5">
+        <v>43385</v>
+      </c>
+      <c r="L4">
         <f t="shared" si="2"/>
-        <v>Last name 3 First name 3</v>
-      </c>
-      <c r="J4">
-        <f t="shared" si="3"/>
-        <v>16988289</v>
-      </c>
-      <c r="K4" s="1">
-        <v>43385</v>
-      </c>
-      <c r="L4">
-        <f t="shared" si="4"/>
         <v>300</v>
       </c>
     </row>
@@ -659,19 +742,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(B$1," ",$A5)</f>
         <v>First name 4</v>
       </c>
       <c r="C5" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C$1," ",$A5)</f>
         <v>Last name 4</v>
       </c>
       <c r="D5" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(D$1," ",$A5)</f>
         <v>Username 4</v>
       </c>
       <c r="E5" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(E$1," ",$A5)</f>
         <v>Address 4</v>
       </c>
       <c r="F5" t="s">
@@ -684,18 +767,18 @@
         <v>6654</v>
       </c>
       <c r="I5" t="str">
+        <f t="shared" si="0"/>
+        <v>Last name 4 First name 4</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="1"/>
+        <v>22651052</v>
+      </c>
+      <c r="K5" s="5">
+        <v>43386</v>
+      </c>
+      <c r="L5">
         <f t="shared" si="2"/>
-        <v>Last name 4 First name 4</v>
-      </c>
-      <c r="J5">
-        <f t="shared" si="3"/>
-        <v>22651052</v>
-      </c>
-      <c r="K5" s="1">
-        <v>43386</v>
-      </c>
-      <c r="L5">
-        <f t="shared" si="4"/>
         <v>400</v>
       </c>
     </row>
@@ -704,19 +787,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(B$1," ",$A6)</f>
         <v>First name 5</v>
       </c>
       <c r="C6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C$1," ",$A6)</f>
         <v>Last name 5</v>
       </c>
       <c r="D6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(D$1," ",$A6)</f>
         <v>Username 5</v>
       </c>
       <c r="E6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(E$1," ",$A6)</f>
         <v>Address 5</v>
       </c>
       <c r="F6" t="s">
@@ -729,18 +812,18 @@
         <v>6655</v>
       </c>
       <c r="I6" t="str">
+        <f t="shared" si="0"/>
+        <v>Last name 5 First name 5</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="1"/>
+        <v>28313815</v>
+      </c>
+      <c r="K6" s="5">
+        <v>43387</v>
+      </c>
+      <c r="L6">
         <f t="shared" si="2"/>
-        <v>Last name 5 First name 5</v>
-      </c>
-      <c r="J6">
-        <f t="shared" si="3"/>
-        <v>28313815</v>
-      </c>
-      <c r="K6" s="1">
-        <v>43387</v>
-      </c>
-      <c r="L6">
-        <f t="shared" si="4"/>
         <v>500</v>
       </c>
     </row>
@@ -749,19 +832,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(B$1," ",$A7)</f>
         <v>First name 6</v>
       </c>
       <c r="C7" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C$1," ",$A7)</f>
         <v>Last name 6</v>
       </c>
       <c r="D7" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(D$1," ",$A7)</f>
         <v>Username 6</v>
       </c>
       <c r="E7" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(E$1," ",$A7)</f>
         <v>Address 6</v>
       </c>
       <c r="F7" t="s">
@@ -774,18 +857,18 @@
         <v>6656</v>
       </c>
       <c r="I7" t="str">
+        <f t="shared" si="0"/>
+        <v>Last name 6 First name 6</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="1"/>
+        <v>33976578</v>
+      </c>
+      <c r="K7" s="5">
+        <v>43388</v>
+      </c>
+      <c r="L7">
         <f t="shared" si="2"/>
-        <v>Last name 6 First name 6</v>
-      </c>
-      <c r="J7">
-        <f t="shared" si="3"/>
-        <v>33976578</v>
-      </c>
-      <c r="K7" s="1">
-        <v>43388</v>
-      </c>
-      <c r="L7">
-        <f t="shared" si="4"/>
         <v>600</v>
       </c>
     </row>
@@ -794,19 +877,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(B$1," ",$A8)</f>
         <v>First name 7</v>
       </c>
       <c r="C8" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C$1," ",$A8)</f>
         <v>Last name 7</v>
       </c>
       <c r="D8" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(D$1," ",$A8)</f>
         <v>Username 7</v>
       </c>
       <c r="E8" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(E$1," ",$A8)</f>
         <v>Address 7</v>
       </c>
       <c r="F8" t="s">
@@ -819,18 +902,18 @@
         <v>6657</v>
       </c>
       <c r="I8" t="str">
+        <f t="shared" si="0"/>
+        <v>Last name 7 First name 7</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="1"/>
+        <v>39639341</v>
+      </c>
+      <c r="K8" s="5">
+        <v>43389</v>
+      </c>
+      <c r="L8">
         <f t="shared" si="2"/>
-        <v>Last name 7 First name 7</v>
-      </c>
-      <c r="J8">
-        <f t="shared" si="3"/>
-        <v>39639341</v>
-      </c>
-      <c r="K8" s="1">
-        <v>43389</v>
-      </c>
-      <c r="L8">
-        <f t="shared" si="4"/>
         <v>700</v>
       </c>
     </row>
@@ -839,19 +922,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(B$1," ",$A9)</f>
         <v>First name 8</v>
       </c>
       <c r="C9" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C$1," ",$A9)</f>
         <v>Last name 8</v>
       </c>
       <c r="D9" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(D$1," ",$A9)</f>
         <v>Username 8</v>
       </c>
       <c r="E9" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(E$1," ",$A9)</f>
         <v>Address 8</v>
       </c>
       <c r="F9" t="s">
@@ -864,18 +947,18 @@
         <v>6658</v>
       </c>
       <c r="I9" t="str">
+        <f t="shared" si="0"/>
+        <v>Last name 8 First name 8</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="1"/>
+        <v>45302104</v>
+      </c>
+      <c r="K9" s="5">
+        <v>43390</v>
+      </c>
+      <c r="L9">
         <f t="shared" si="2"/>
-        <v>Last name 8 First name 8</v>
-      </c>
-      <c r="J9">
-        <f t="shared" si="3"/>
-        <v>45302104</v>
-      </c>
-      <c r="K9" s="1">
-        <v>43390</v>
-      </c>
-      <c r="L9">
-        <f t="shared" si="4"/>
         <v>800</v>
       </c>
     </row>
@@ -884,19 +967,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(B$1," ",$A10)</f>
         <v>First name 9</v>
       </c>
       <c r="C10" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C$1," ",$A10)</f>
         <v>Last name 9</v>
       </c>
       <c r="D10" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(D$1," ",$A10)</f>
         <v>Username 9</v>
       </c>
       <c r="E10" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(E$1," ",$A10)</f>
         <v>Address 9</v>
       </c>
       <c r="F10" t="s">
@@ -909,18 +992,18 @@
         <v>6659</v>
       </c>
       <c r="I10" t="str">
+        <f t="shared" si="0"/>
+        <v>Last name 9 First name 9</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="1"/>
+        <v>50964867</v>
+      </c>
+      <c r="K10" s="5">
+        <v>43391</v>
+      </c>
+      <c r="L10">
         <f t="shared" si="2"/>
-        <v>Last name 9 First name 9</v>
-      </c>
-      <c r="J10">
-        <f t="shared" si="3"/>
-        <v>50964867</v>
-      </c>
-      <c r="K10" s="1">
-        <v>43391</v>
-      </c>
-      <c r="L10">
-        <f t="shared" si="4"/>
         <v>900</v>
       </c>
     </row>
@@ -929,19 +1012,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(B$1," ",$A11)</f>
         <v>First name 10</v>
       </c>
       <c r="C11" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C$1," ",$A11)</f>
         <v>Last name 10</v>
       </c>
       <c r="D11" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(D$1," ",$A11)</f>
         <v>Username 10</v>
       </c>
       <c r="E11" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(E$1," ",$A11)</f>
         <v>Address 10</v>
       </c>
       <c r="F11" t="s">
@@ -954,18 +1037,18 @@
         <v>6660</v>
       </c>
       <c r="I11" t="str">
+        <f t="shared" si="0"/>
+        <v>Last name 10 First name 10</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="1"/>
+        <v>56627630</v>
+      </c>
+      <c r="K11" s="5">
+        <v>43392</v>
+      </c>
+      <c r="L11">
         <f t="shared" si="2"/>
-        <v>Last name 10 First name 10</v>
-      </c>
-      <c r="J11">
-        <f t="shared" si="3"/>
-        <v>56627630</v>
-      </c>
-      <c r="K11" s="1">
-        <v>43392</v>
-      </c>
-      <c r="L11">
-        <f t="shared" si="4"/>
         <v>1000</v>
       </c>
     </row>
@@ -974,19 +1057,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(B$1," ",$A12)</f>
         <v>First name 11</v>
       </c>
       <c r="C12" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C$1," ",$A12)</f>
         <v>Last name 11</v>
       </c>
       <c r="D12" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(D$1," ",$A12)</f>
         <v>Username 11</v>
       </c>
       <c r="E12" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(E$1," ",$A12)</f>
         <v>Address 11</v>
       </c>
       <c r="F12" t="s">
@@ -999,18 +1082,18 @@
         <v>6661</v>
       </c>
       <c r="I12" t="str">
+        <f t="shared" si="0"/>
+        <v>Last name 11 First name 11</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="1"/>
+        <v>62290393</v>
+      </c>
+      <c r="K12" s="5">
+        <v>43393</v>
+      </c>
+      <c r="L12">
         <f t="shared" si="2"/>
-        <v>Last name 11 First name 11</v>
-      </c>
-      <c r="J12">
-        <f t="shared" si="3"/>
-        <v>62290393</v>
-      </c>
-      <c r="K12" s="1">
-        <v>43393</v>
-      </c>
-      <c r="L12">
-        <f t="shared" si="4"/>
         <v>1100</v>
       </c>
     </row>
@@ -1019,19 +1102,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(B$1," ",$A13)</f>
         <v>First name 12</v>
       </c>
       <c r="C13" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C$1," ",$A13)</f>
         <v>Last name 12</v>
       </c>
       <c r="D13" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(D$1," ",$A13)</f>
         <v>Username 12</v>
       </c>
       <c r="E13" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(E$1," ",$A13)</f>
         <v>Address 12</v>
       </c>
       <c r="F13" t="s">
@@ -1044,18 +1127,18 @@
         <v>6662</v>
       </c>
       <c r="I13" t="str">
+        <f t="shared" si="0"/>
+        <v>Last name 12 First name 12</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="1"/>
+        <v>67953156</v>
+      </c>
+      <c r="K13" s="5">
+        <v>43394</v>
+      </c>
+      <c r="L13">
         <f t="shared" si="2"/>
-        <v>Last name 12 First name 12</v>
-      </c>
-      <c r="J13">
-        <f t="shared" si="3"/>
-        <v>67953156</v>
-      </c>
-      <c r="K13" s="1">
-        <v>43394</v>
-      </c>
-      <c r="L13">
-        <f t="shared" si="4"/>
         <v>1200</v>
       </c>
     </row>
@@ -1064,19 +1147,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(B$1," ",$A14)</f>
         <v>First name 13</v>
       </c>
       <c r="C14" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C$1," ",$A14)</f>
         <v>Last name 13</v>
       </c>
       <c r="D14" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(D$1," ",$A14)</f>
         <v>Username 13</v>
       </c>
       <c r="E14" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(E$1," ",$A14)</f>
         <v>Address 13</v>
       </c>
       <c r="F14" t="s">
@@ -1089,18 +1172,18 @@
         <v>6663</v>
       </c>
       <c r="I14" t="str">
+        <f t="shared" si="0"/>
+        <v>Last name 13 First name 13</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="1"/>
+        <v>73615919</v>
+      </c>
+      <c r="K14" s="5">
+        <v>43395</v>
+      </c>
+      <c r="L14">
         <f t="shared" si="2"/>
-        <v>Last name 13 First name 13</v>
-      </c>
-      <c r="J14">
-        <f t="shared" si="3"/>
-        <v>73615919</v>
-      </c>
-      <c r="K14" s="1">
-        <v>43395</v>
-      </c>
-      <c r="L14">
-        <f t="shared" si="4"/>
         <v>1300</v>
       </c>
     </row>
@@ -1109,19 +1192,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(B$1," ",$A15)</f>
         <v>First name 14</v>
       </c>
       <c r="C15" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C$1," ",$A15)</f>
         <v>Last name 14</v>
       </c>
       <c r="D15" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(D$1," ",$A15)</f>
         <v>Username 14</v>
       </c>
       <c r="E15" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(E$1," ",$A15)</f>
         <v>Address 14</v>
       </c>
       <c r="F15" t="s">
@@ -1134,18 +1217,18 @@
         <v>6664</v>
       </c>
       <c r="I15" t="str">
+        <f t="shared" si="0"/>
+        <v>Last name 14 First name 14</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="1"/>
+        <v>79278682</v>
+      </c>
+      <c r="K15" s="5">
+        <v>43396</v>
+      </c>
+      <c r="L15">
         <f t="shared" si="2"/>
-        <v>Last name 14 First name 14</v>
-      </c>
-      <c r="J15">
-        <f t="shared" si="3"/>
-        <v>79278682</v>
-      </c>
-      <c r="K15" s="1">
-        <v>43396</v>
-      </c>
-      <c r="L15">
-        <f t="shared" si="4"/>
         <v>1400</v>
       </c>
     </row>
@@ -1154,19 +1237,19 @@
         <v>15</v>
       </c>
       <c r="B16" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(B$1," ",$A16)</f>
         <v>First name 15</v>
       </c>
       <c r="C16" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C$1," ",$A16)</f>
         <v>Last name 15</v>
       </c>
       <c r="D16" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(D$1," ",$A16)</f>
         <v>Username 15</v>
       </c>
       <c r="E16" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(E$1," ",$A16)</f>
         <v>Address 15</v>
       </c>
       <c r="F16" t="s">
@@ -1179,18 +1262,18 @@
         <v>6665</v>
       </c>
       <c r="I16" t="str">
+        <f t="shared" si="0"/>
+        <v>Last name 15 First name 15</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="1"/>
+        <v>84941445</v>
+      </c>
+      <c r="K16" s="5">
+        <v>43397</v>
+      </c>
+      <c r="L16">
         <f t="shared" si="2"/>
-        <v>Last name 15 First name 15</v>
-      </c>
-      <c r="J16">
-        <f t="shared" si="3"/>
-        <v>84941445</v>
-      </c>
-      <c r="K16" s="1">
-        <v>43397</v>
-      </c>
-      <c r="L16">
-        <f t="shared" si="4"/>
         <v>1500</v>
       </c>
     </row>
@@ -1199,19 +1282,19 @@
         <v>16</v>
       </c>
       <c r="B17" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(B$1," ",$A17)</f>
         <v>First name 16</v>
       </c>
       <c r="C17" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C$1," ",$A17)</f>
         <v>Last name 16</v>
       </c>
       <c r="D17" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(D$1," ",$A17)</f>
         <v>Username 16</v>
       </c>
       <c r="E17" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(E$1," ",$A17)</f>
         <v>Address 16</v>
       </c>
       <c r="F17" t="s">
@@ -1224,18 +1307,18 @@
         <v>6666</v>
       </c>
       <c r="I17" t="str">
+        <f t="shared" si="0"/>
+        <v>Last name 16 First name 16</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="1"/>
+        <v>90604208</v>
+      </c>
+      <c r="K17" s="5">
+        <v>43398</v>
+      </c>
+      <c r="L17">
         <f t="shared" si="2"/>
-        <v>Last name 16 First name 16</v>
-      </c>
-      <c r="J17">
-        <f t="shared" si="3"/>
-        <v>90604208</v>
-      </c>
-      <c r="K17" s="1">
-        <v>43398</v>
-      </c>
-      <c r="L17">
-        <f t="shared" si="4"/>
         <v>1600</v>
       </c>
     </row>
@@ -1244,19 +1327,19 @@
         <v>17</v>
       </c>
       <c r="B18" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(B$1," ",$A18)</f>
         <v>First name 17</v>
       </c>
       <c r="C18" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(C$1," ",$A18)</f>
         <v>Last name 17</v>
       </c>
       <c r="D18" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(D$1," ",$A18)</f>
         <v>Username 17</v>
       </c>
       <c r="E18" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(E$1," ",$A18)</f>
         <v>Address 17</v>
       </c>
       <c r="F18" t="s">
@@ -1269,18 +1352,18 @@
         <v>6667</v>
       </c>
       <c r="I18" t="str">
+        <f t="shared" si="0"/>
+        <v>Last name 17 First name 17</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="1"/>
+        <v>96266971</v>
+      </c>
+      <c r="K18" s="5">
+        <v>43399</v>
+      </c>
+      <c r="L18">
         <f t="shared" si="2"/>
-        <v>Last name 17 First name 17</v>
-      </c>
-      <c r="J18">
-        <f t="shared" si="3"/>
-        <v>96266971</v>
-      </c>
-      <c r="K18" s="1">
-        <v>43399</v>
-      </c>
-      <c r="L18">
-        <f t="shared" si="4"/>
         <v>1700</v>
       </c>
     </row>
@@ -1289,19 +1372,19 @@
         <v>18</v>
       </c>
       <c r="B19" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(B$1," ",$A19)</f>
         <v>First name 18</v>
       </c>
       <c r="C19" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(C$1," ",$A19)</f>
         <v>Last name 18</v>
       </c>
       <c r="D19" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(D$1," ",$A19)</f>
         <v>Username 18</v>
       </c>
       <c r="E19" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(E$1," ",$A19)</f>
         <v>Address 18</v>
       </c>
       <c r="F19" t="s">
@@ -1314,18 +1397,18 @@
         <v>6668</v>
       </c>
       <c r="I19" t="str">
+        <f t="shared" si="0"/>
+        <v>Last name 18 First name 18</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="1"/>
+        <v>101929734</v>
+      </c>
+      <c r="K19" s="5">
+        <v>43400</v>
+      </c>
+      <c r="L19">
         <f t="shared" si="2"/>
-        <v>Last name 18 First name 18</v>
-      </c>
-      <c r="J19">
-        <f t="shared" si="3"/>
-        <v>101929734</v>
-      </c>
-      <c r="K19" s="1">
-        <v>43400</v>
-      </c>
-      <c r="L19">
-        <f t="shared" si="4"/>
         <v>1800</v>
       </c>
     </row>
@@ -1334,19 +1417,19 @@
         <v>19</v>
       </c>
       <c r="B20" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(B$1," ",$A20)</f>
         <v>First name 19</v>
       </c>
       <c r="C20" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(C$1," ",$A20)</f>
         <v>Last name 19</v>
       </c>
       <c r="D20" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(D$1," ",$A20)</f>
         <v>Username 19</v>
       </c>
       <c r="E20" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(E$1," ",$A20)</f>
         <v>Address 19</v>
       </c>
       <c r="F20" t="s">
@@ -1359,19 +1442,331 @@
         <v>6669</v>
       </c>
       <c r="I20" t="str">
+        <f t="shared" si="0"/>
+        <v>Last name 19 First name 19</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="1"/>
+        <v>107592497</v>
+      </c>
+      <c r="K20" s="5">
+        <v>43401</v>
+      </c>
+      <c r="L20">
         <f t="shared" si="2"/>
-        <v>Last name 19 First name 19</v>
-      </c>
-      <c r="J20">
-        <f t="shared" si="3"/>
-        <v>107592497</v>
-      </c>
-      <c r="K20" s="1">
-        <v>43401</v>
-      </c>
-      <c r="L20">
-        <f t="shared" si="4"/>
         <v>1900</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="str">
+        <f>_xlfn.CONCAT(B$1," ",$A21)</f>
+        <v>First name 20</v>
+      </c>
+      <c r="C21" t="str">
+        <f>_xlfn.CONCAT(C$1," ",$A21)</f>
+        <v>Last name 20</v>
+      </c>
+      <c r="D21" t="str">
+        <f>_xlfn.CONCAT(D$1," ",$A21)</f>
+        <v>Username 20</v>
+      </c>
+      <c r="E21" t="str">
+        <f>_xlfn.CONCAT(E$1," ",$A21)</f>
+        <v>Address 20</v>
+      </c>
+      <c r="F21" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21">
+        <v>6670</v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" ref="I21" si="3">_xlfn.CONCAT(C21," ",B21)</f>
+        <v>Last name 20 First name 20</v>
+      </c>
+      <c r="J21">
+        <f t="shared" ref="J21" si="4">A21*5662763</f>
+        <v>113255260</v>
+      </c>
+      <c r="K21" s="5">
+        <v>43402</v>
+      </c>
+      <c r="L21">
+        <f t="shared" ref="L21" si="5">A21*100</f>
+        <v>2000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF1977FC-C3CB-4E35-BFE3-4E3A78CD0FA7}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="11.53125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.9296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.3984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.796875" style="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>20</v>
+      </c>
+      <c r="C2" s="3">
+        <v>3.2638888888888891E-2</v>
+      </c>
+      <c r="D2">
+        <f>47/B2</f>
+        <v>2.35</v>
+      </c>
+      <c r="E2" s="3">
+        <v>3.7499999999999999E-2</v>
+      </c>
+      <c r="F2">
+        <f>54/B2</f>
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+      <c r="C3" s="3">
+        <v>2.361111111111111E-2</v>
+      </c>
+      <c r="D3">
+        <f>34/B3</f>
+        <v>1.7</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1.3194444444444444E-2</v>
+      </c>
+      <c r="F3">
+        <f>19/B3</f>
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>20</v>
+      </c>
+      <c r="C4" s="3">
+        <v>2.9861111111111113E-2</v>
+      </c>
+      <c r="D4">
+        <f>43/B4</f>
+        <v>2.15</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="F4">
+        <f>24/B4</f>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>50</v>
+      </c>
+      <c r="C5" s="3">
+        <v>7.3611111111111113E-2</v>
+      </c>
+      <c r="D5">
+        <f>(60+46)/B5</f>
+        <v>2.12</v>
+      </c>
+      <c r="E5" s="3">
+        <v>5.486111111111111E-2</v>
+      </c>
+      <c r="F5">
+        <f>79/B5</f>
+        <v>1.58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>50</v>
+      </c>
+      <c r="C6" s="3">
+        <v>4.3750000000000004E-2</v>
+      </c>
+      <c r="D6">
+        <f>63/B6</f>
+        <v>1.26</v>
+      </c>
+      <c r="E6" s="3">
+        <v>2.8472222222222222E-2</v>
+      </c>
+      <c r="F6">
+        <f>41/B6</f>
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>50</v>
+      </c>
+      <c r="C7" s="3">
+        <v>5.2777777777777778E-2</v>
+      </c>
+      <c r="D7">
+        <f>76/B7</f>
+        <v>1.52</v>
+      </c>
+      <c r="E7" s="3">
+        <v>3.0555555555555555E-2</v>
+      </c>
+      <c r="F7">
+        <f>44/B7</f>
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>100</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.14305555555555557</v>
+      </c>
+      <c r="D8">
+        <f>(3*60 +26)/B8</f>
+        <v>2.06</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="F8">
+        <f>150/B8</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>100</v>
+      </c>
+      <c r="C9" s="3">
+        <v>8.6805555555555566E-2</v>
+      </c>
+      <c r="D9">
+        <f>125/B9</f>
+        <v>1.25</v>
+      </c>
+      <c r="E9" s="3">
+        <v>5.6944444444444443E-2</v>
+      </c>
+      <c r="F9">
+        <f>82/B9</f>
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>100</v>
+      </c>
+      <c r="C10" s="3">
+        <v>8.7500000000000008E-2</v>
+      </c>
+      <c r="D10">
+        <f>126/B10</f>
+        <v>1.26</v>
+      </c>
+      <c r="E10" s="3">
+        <v>5.6250000000000001E-2</v>
+      </c>
+      <c r="F10">
+        <f>81/B10</f>
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>100</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.11319444444444444</v>
+      </c>
+      <c r="D11">
+        <f>(120+43)/B11</f>
+        <v>1.63</v>
+      </c>
+      <c r="E11" s="3">
+        <v>6.8749999999999992E-2</v>
+      </c>
+      <c r="F11">
+        <f>99/B11</f>
+        <v>0.99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>